<commit_message>
Atualização automática de RIO_PARDO.xlsx
</commit_message>
<xml_diff>
--- a/RIO_PARDO.xlsx
+++ b/RIO_PARDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F501D1B6-99F2-4D0C-BBF0-AFA9224D369C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C99A81C-1C5E-4E3D-B4D2-88AC759E2EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1288,7 +1288,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{34913C5B-986C-4F07-A112-451EEEFB1332}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{DBB19184-4A54-441F-923F-BA413AF4412A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1318,10 +1318,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E393C56-C931-4323-B2DE-E78593A513DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BF01F59-8F57-4F94-9122-628B594226BE}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1359,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCACDA5F-0ABB-4AAE-AE15-06BFA4C90615}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F0AD44B-93F2-412D-AE92-C5F8DC16124B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1422,7 +1422,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{279D38A2-35B8-46FF-87CD-1EAAA3939F9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7989037-7433-4B95-9130-7CEB6E1FD73C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1441,7 +1441,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCAF9FA4-EE67-499B-DFC6-971D4343832E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C937458-914B-92A0-8DAA-A6F4736D9DCF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1490,7 +1490,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8399BEF6-92A4-BF4C-CAEC-F81F73386207}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{003C72C7-5D68-30AA-3EAD-9F8F560E6AD6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1509,7 +1509,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB61EF6A-C147-F97D-7D49-208633679BD8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD8DD8F2-464E-CD54-635A-22A7635F8B24}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1540,7 +1540,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5A557A3-5C18-7080-CE8C-F39834FEE0A2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4D23EAC-F415-560E-E434-FDF5FA729BF4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1571,7 +1571,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7619322E-C146-9F14-5FC4-2D7E8AAB7B2D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CEA0051-D786-B52D-0056-5DF06C9379CC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1614,7 +1614,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCE98FC1-FDA2-44E6-B760-8BE055E0964A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E75D3899-9D97-4E13-921D-80FB68F8100C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1652,7 +1652,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F9CD4DF-0D18-44E0-A266-701C26175348}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14FEE521-7CD1-4888-A8D5-A4201065B494}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1695,7 +1695,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43C6E5EB-C252-454E-B9CB-282626B2B9ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C1D88E4-DB91-4B69-90BF-48EFDEDC3D8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2008,7 +2008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB27BD6-FDCB-4116-A6BB-D71503E79DC2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EE1E92-7DD6-471D-AF94-B3E857AC02EB}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>